<commit_message>
Renamed Categories to more user- friendly words.i.e. more easier to understand
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeko\Documents\work\SourceWork\HackManchester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceControl\HackManchester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,28 +53,28 @@
     <t>Visual Basic</t>
   </si>
   <si>
-    <t>Feature Renaming</t>
-  </si>
-  <si>
-    <t>Garbage Collection</t>
-  </si>
-  <si>
-    <t>Class Variables / Methods</t>
-  </si>
-  <si>
-    <t>Regular Expressions</t>
-  </si>
-  <si>
     <t>Language Integration</t>
   </si>
   <si>
     <t>Built-In Security</t>
+  </si>
+  <si>
+    <t>Renaming Feature</t>
+  </si>
+  <si>
+    <t>Memory Management</t>
+  </si>
+  <si>
+    <t>Variables &amp; Classes</t>
+  </si>
+  <si>
+    <t>Validation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,30 +464,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="29.25" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -718,7 +722,7 @@
       <c r="U7"/>
       <c r="V7"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added a new category and updated from yes - no to numbers
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Eiffel</t>
   </si>
@@ -53,22 +53,52 @@
     <t>Visual Basic</t>
   </si>
   <si>
+    <t>Garbage Collection</t>
+  </si>
+  <si>
+    <t>Regular Expressions</t>
+  </si>
+  <si>
     <t>Language Integration</t>
   </si>
   <si>
     <t>Built-In Security</t>
   </si>
   <si>
-    <t>Renaming Feature</t>
-  </si>
-  <si>
-    <t>Memory Management</t>
-  </si>
-  <si>
     <t>Variables &amp; Classes</t>
   </si>
   <si>
-    <t>Validation</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>Java Script</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>Haskell</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Scala</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Objective C</t>
+  </si>
+  <si>
+    <t>Method Overloading</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
   </si>
 </sst>
 </file>
@@ -110,7 +140,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +150,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -148,6 +184,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,36 +499,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -499,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
@@ -516,8 +559,10 @@
       <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="H2"/>
-      <c r="I2"/>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -537,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
@@ -546,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -554,7 +599,9 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-      <c r="H3"/>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -584,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
         <v>3</v>
@@ -592,7 +639,9 @@
       <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="H4"/>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
@@ -622,7 +671,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -660,7 +709,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F6" s="4">
         <v>4</v>
@@ -698,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4">
         <v>2</v>
@@ -736,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
         <v>3</v>
@@ -782,13 +831,87 @@
         <v>0</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more correct numbers and fixing categories
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -502,7 +502,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
@@ -642,7 +642,7 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" s="5"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -662,25 +662,27 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
       </c>
       <c r="D5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4">
         <v>4</v>
       </c>
       <c r="F5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5"/>
-      <c r="I5"/>
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -700,13 +702,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4">
         <v>4</v>
@@ -715,10 +717,12 @@
         <v>4</v>
       </c>
       <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6"/>
-      <c r="I6"/>
+        <v>3</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -738,13 +742,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4">
         <v>3</v>
@@ -782,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <v>3</v>

</xml_diff>

<commit_message>
Completed ;     C++,     Python,     Perl
N.B. Green boxes shows its completed
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -502,7 +502,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,8 +759,10 @@
       <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7"/>
-      <c r="I7"/>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -780,7 +782,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -797,22 +799,26 @@
       <c r="G8" s="4">
         <v>0</v>
       </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
       </c>
       <c r="E9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
@@ -820,6 +826,10 @@
       <c r="G9" s="4">
         <v>1</v>
       </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:22" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
complete;   Visual Basic   C   PHP
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -502,7 +502,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,13 +836,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="4">
         <v>3</v>
@@ -853,22 +853,45 @@
       <c r="G10" s="4">
         <v>0</v>
       </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
       <c r="C11" s="4">
         <v>4</v>
       </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
       <c r="E11" s="4">
         <v>4</v>
       </c>
+      <c r="F11" s="4">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3</v>
+      </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
       <c r="C12" s="4">
         <v>2</v>
       </c>
@@ -884,6 +907,10 @@
       <c r="G12" s="4">
         <v>2</v>
       </c>
+      <c r="H12" s="4">
+        <v>2</v>
+      </c>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">

</xml_diff>

<commit_message>
Completed entering all data into table
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,11 +1093,55 @@
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2</v>
+      </c>
+      <c r="J20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Spreadsheet and all logos are downloaded and edited
</commit_message>
<xml_diff>
--- a/CardData2ndDraft.xlsx
+++ b/CardData2ndDraft.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Eiffel</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Clojure</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +516,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +582,9 @@
       <c r="I2" s="4">
         <v>0</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
@@ -617,7 +624,9 @@
       <c r="I3" s="4">
         <v>0</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
@@ -657,7 +666,9 @@
       <c r="I4" s="4">
         <v>0</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -697,7 +708,9 @@
       <c r="I5" s="4">
         <v>2</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
@@ -737,7 +750,9 @@
       <c r="I6" s="4">
         <v>2</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
@@ -777,7 +792,9 @@
       <c r="I7" s="4">
         <v>2</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
@@ -817,7 +834,9 @@
       <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -844,7 +863,9 @@
       <c r="I9" s="4">
         <v>0</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -871,7 +892,9 @@
       <c r="I10" s="4">
         <v>0</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -898,7 +921,9 @@
       <c r="I11" s="4">
         <v>3</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -925,7 +950,9 @@
       <c r="I12" s="4">
         <v>2</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -952,7 +979,9 @@
       <c r="I13" s="4">
         <v>2</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -979,7 +1008,9 @@
       <c r="I14" s="4">
         <v>1</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -1006,7 +1037,9 @@
       <c r="I15" s="4">
         <v>2</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -1033,7 +1066,9 @@
       <c r="I16" s="4">
         <v>1</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1060,7 +1095,9 @@
       <c r="I17" s="4">
         <v>1</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="J17" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -1087,7 +1124,9 @@
       <c r="I18" s="4">
         <v>0</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -1114,7 +1153,9 @@
       <c r="I19" s="4">
         <v>2</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -1141,7 +1182,9 @@
       <c r="I20" s="4">
         <v>2</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>